<commit_message>
add February 2025 events and update residents directory
</commit_message>
<xml_diff>
--- a/3-1-heritage/0-heritage-happenings/2025/03-march/resident-directory/2025-03-heritage-resident-directory.xlsx
+++ b/3-1-heritage/0-heritage-happenings/2025/03-march/resident-directory/2025-03-heritage-resident-directory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4348e1419f457eb2/Documents/GitHub/theo-armour-agenda/3-1-heritage/0-heritage-happenings/2025/03-march/resident-directory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="833" documentId="8_{47523533-A004-48EF-BEEC-0FA3DE3C4717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE3E1E78-6915-4C8B-BFD5-4CE86D1E2057}"/>
+  <xr:revisionPtr revIDLastSave="835" documentId="8_{47523533-A004-48EF-BEEC-0FA3DE3C4717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4973FFAA-9639-4857-868E-5E162EDF7C06}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="754" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1693" uniqueCount="1103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1694" uniqueCount="1104">
   <si>
     <t>First Name</t>
   </si>
@@ -3379,6 +3379,9 @@
   </si>
   <si>
     <t>gary@seniordoc.com</t>
+  </si>
+  <si>
+    <t>mchurch@felton.org</t>
   </si>
 </sst>
 </file>
@@ -3986,6 +3989,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -9757,7 +9764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C4F1CA-A107-47E1-B61D-684F7BB5060E}">
   <dimension ref="A1:Z173"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" showRuler="0" view="pageLayout" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" showZeros="0" showRuler="0" view="pageLayout" topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
@@ -16076,7 +16083,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23046875" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -16125,6 +16132,9 @@
       <c r="B3" s="11" t="s">
         <v>1098</v>
       </c>
+      <c r="C3" s="11" t="s">
+        <v>1103</v>
+      </c>
       <c r="D3" s="11" t="s">
         <v>1074</v>
       </c>

</xml_diff>